<commit_message>
updates to README, Bill of Materials, and remove some debug code from ProcessingGUI
</commit_message>
<xml_diff>
--- a/Pneumatic System Bill of Materials.xlsx
+++ b/Pneumatic System Bill of Materials.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\MillerLab\Pneumatics Github\OpenSourcePneumaticSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/b/G3_Docs/Professor/2013 Rice Bioe/GITHUB/OpenSourcePneumaticSystem/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="5772"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33120" windowHeight="22660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -167,12 +170,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +241,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -265,7 +274,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -628,34 +637,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" style="1" customWidth="1"/>
-    <col min="6" max="7" width="15.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="46.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="80.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="9.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -681,7 +690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -708,7 +717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -728,14 +737,14 @@
         <v>1</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G15" si="0">F4*E4</f>
+        <f t="shared" ref="G4:G13" si="0">F4*E4</f>
         <v>398</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -762,7 +771,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -789,7 +798,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F7" s="10" t="s">
         <v>4</v>
       </c>
@@ -798,13 +807,13 @@
         <v>573.80000000000007</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -829,7 +838,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -856,7 +865,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -883,7 +892,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -910,7 +919,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -937,7 +946,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F14" s="10" t="s">
         <v>24</v>
       </c>
@@ -946,25 +955,26 @@
         <v>1201.48</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G15" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1"/>
     <hyperlink ref="B12" r:id="rId2"/>
@@ -977,6 +987,6 @@
     <hyperlink ref="B3" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="51" orientation="landscape" r:id="rId10"/>
+  <pageSetup scale="50" orientation="landscape" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>